<commit_message>
Fix URN & Typo
An URN was accidentally modified in PR #2229 on the last commit. This fix reverts to the original URN and also fixes a typo in requirement 2.1.2.g.
</commit_message>
<xml_diff>
--- a/tools/excel/NIS2/Annex-Implementing-Regulation-of-NIS2-on-T-M.xlsx
+++ b/tools/excel/NIS2/Annex-Implementing-Regulation-of-NIS2-on-T-M.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\NIS2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B104D80-BA8C-4948-826F-4C653ECA1F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F8105F-B2A6-422B-982F-E4B076F24279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8440" yWindow="-18080" windowWidth="25450" windowHeight="16320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3056" uniqueCount="2628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3057" uniqueCount="2629">
   <si>
     <t>type</t>
   </si>
@@ -8056,6 +8056,9 @@
   </si>
   <si>
     <t>12.5.1</t>
+  </si>
+  <si>
+    <t>2.1.2.g</t>
   </si>
 </sst>
 </file>
@@ -8538,7 +8541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -8569,7 +8572,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="22">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -8864,9 +8867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N440"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A410" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E414" sqref="E414"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -9801,7 +9804,10 @@
       <c r="B34">
         <v>4</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="23" t="s">
+        <v>2628</v>
+      </c>
+      <c r="D34" s="24" t="s">
         <v>239</v>
       </c>
       <c r="F34" s="10" t="s">

</xml_diff>